<commit_message>
JavaScripts Notes (Lectures) + Logs Update
</commit_message>
<xml_diff>
--- a/Logs/3rd Week Logs.xlsx
+++ b/Logs/3rd Week Logs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3211337A-9391-4D23-A5B1-D4C8754AEB66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9106203-F896-41CC-9814-88F170213BAF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2364" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,7 +1058,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="8">
-        <v>43504</v>
+        <v>43511</v>
       </c>
       <c r="D10" s="16">
         <v>0.41666666666666669</v>
@@ -1083,18 +1083,32 @@
       <c r="B11" s="40">
         <v>4</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="C11" s="8">
+        <v>43511</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="23"/>
+      <c r="G11" s="14">
+        <v>80</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="43"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="40"/>
+      <c r="B12" s="40">
+        <v>5</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1199,7 +1213,7 @@
       </c>
       <c r="G20" s="20">
         <f>SUM(G8:G19)</f>
-        <v>305</v>
+        <v>385</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>

</xml_diff>

<commit_message>
28-30 Lectures JS + Logs
</commit_message>
<xml_diff>
--- a/Logs/3rd Week Logs.xlsx
+++ b/Logs/3rd Week Logs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E51E8A-23D3-45E2-8607-E77CBCDA7443}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856BCD39-226D-448E-9A01-201267CFB814}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2364" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9948" yWindow="1356" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -896,7 +896,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,11 +1116,11 @@
         <v>0.59722222222222221</v>
       </c>
       <c r="E12" s="16">
-        <v>0.72916666666666663</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="14">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>10</v>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="G20" s="20">
         <f>SUM(G8:G19)</f>
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>

</xml_diff>

<commit_message>
JS Lectures DONE! + Logs
</commit_message>
<xml_diff>
--- a/Logs/3rd Week Logs.xlsx
+++ b/Logs/3rd Week Logs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856BCD39-226D-448E-9A01-201267CFB814}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E123D6F5-9ADD-43E9-AA12-1CAA3EE3F83E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9948" yWindow="1356" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3936" yWindow="2352" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -896,7 +896,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,13 +1135,25 @@
       <c r="B13" s="40">
         <v>6</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+      <c r="C13" s="8">
+        <v>43514</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.75347222222222221</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.98958333333333337</v>
+      </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="23"/>
+      <c r="G13" s="14">
+        <v>280</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="J13" s="4"/>
       <c r="K13" s="43"/>
     </row>
@@ -1227,7 +1239,7 @@
       </c>
       <c r="G20" s="20">
         <f>SUM(G8:G19)</f>
-        <v>565</v>
+        <v>845</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>

</xml_diff>